<commit_message>
Removed dictionary from class
functions now edit the dataframe
</commit_message>
<xml_diff>
--- a/user_input/JB0001175447-1_Appendix A Field Survey.xlsx
+++ b/user_input/JB0001175447-1_Appendix A Field Survey.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\2022 Booker Engineering\CLIENTS\CABLECOM\POLE PERMITS\ANACORTES\JB0001175447_PSE_Pole Permit\JB0001175447-1_PSE_Application Attachment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/04ef7c6c9ce6ee46/Documents/GitHub/pole-permit-spreadsheet/user_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5D0A31-FCCE-4EAF-8FEB-A437EC0B96EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2190" yWindow="990" windowWidth="21420" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proposed Appendix A" sheetId="1" r:id="rId1"/>
@@ -1129,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC999"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add data to spreadsheet
</commit_message>
<xml_diff>
--- a/user_input/JB0001175447-1_Appendix A Field Survey.xlsx
+++ b/user_input/JB0001175447-1_Appendix A Field Survey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/04ef7c6c9ce6ee46/Documents/GitHub/pole-permit-spreadsheet/user_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5D0A31-FCCE-4EAF-8FEB-A437EC0B96EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{7C5D0A31-FCCE-4EAF-8FEB-A437EC0B96EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D6CEE43-59FC-47C1-9FB9-E4FE474B781B}"/>
   <bookViews>
-    <workbookView xWindow="3270" yWindow="1905" windowWidth="21420" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2385" yWindow="1470" windowWidth="21420" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proposed Appendix A" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="120">
   <si>
     <t>Wireline Joint Use - Appendix A</t>
   </si>
@@ -237,9 +237,6 @@
   </si>
   <si>
     <t>Anacortes</t>
-  </si>
-  <si>
-    <t>33' 11''</t>
   </si>
   <si>
     <t>CATV 2nd attach: 22' 01''
@@ -270,51 +267,30 @@
     <t>Dress drip loop, Lower CATV to 25' 06''</t>
   </si>
   <si>
-    <t>25' 06''</t>
-  </si>
-  <si>
     <t>Dress drip loop, Lower CATV to 24' 11'', Telco to 23' 11''</t>
   </si>
   <si>
     <t>Lower CATV to 21' 08'', Telco to 20' 08''</t>
   </si>
   <si>
-    <t>21' 08''</t>
-  </si>
-  <si>
-    <t>24' 11''</t>
-  </si>
-  <si>
     <t>Raise Secondary to 25' 00'', Dress drip loop</t>
   </si>
   <si>
     <t>Lower CATV to 23' 04'', Telco to 22' 04''</t>
   </si>
   <si>
-    <t>23' 04''</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lower Fiber to 22' 01'', CATV to 21' 01'', Telco to 20' 01'', Dress drip loop </t>
   </si>
   <si>
-    <t>21' 01''</t>
-  </si>
-  <si>
     <t>Raise Fiber to 25' 09''</t>
   </si>
   <si>
     <t>Lower Fiber to 22' 04''. CATV to 21' 04'', Telco to 20' 04''</t>
   </si>
   <si>
-    <t>21' 04''</t>
-  </si>
-  <si>
     <t>Lower CATV to 22' 04'', Telco to 21' 04''</t>
   </si>
   <si>
-    <t>22' 04''</t>
-  </si>
-  <si>
     <t>Lower CATV to 24' 08'', Telco to 23' 08''</t>
   </si>
   <si>
@@ -336,19 +312,10 @@
     <t>Lower Fiber to 17' 08'', CATV to 16' 08'', Ground Streetlight</t>
   </si>
   <si>
-    <t>16' 08''</t>
-  </si>
-  <si>
     <t>Lower Fiber to 19' 04'', CATV to 18' 04'', Ground Streetlight</t>
   </si>
   <si>
-    <t>18' 04''</t>
-  </si>
-  <si>
     <t>Lower CATV to 20' 00'', Telco to 19' 00''</t>
-  </si>
-  <si>
-    <t>20' 00''</t>
   </si>
   <si>
     <t>Dress drip loop, Telco to 21' 11''</t>
@@ -427,9 +394,6 @@
   </si>
   <si>
     <t>-122.606704</t>
-  </si>
-  <si>
-    <t>21' 00"</t>
   </si>
   <si>
     <t>Lower CATV to 21' 00"
@@ -1129,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC999"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1459,7 +1423,7 @@
         <v>27</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="F10" s="16">
         <v>48.430056</v>
@@ -1474,25 +1438,25 @@
         <v>3400</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K10" s="17">
         <v>3304</v>
       </c>
-      <c r="L10" s="17" t="s">
-        <v>67</v>
+      <c r="L10" s="17">
+        <v>3311</v>
       </c>
       <c r="M10" s="17">
         <v>3404</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O10" s="17">
         <v>2802</v>
       </c>
       <c r="P10" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q10" s="17">
         <v>2702</v>
@@ -1501,16 +1465,16 @@
         <v>2802</v>
       </c>
       <c r="S10" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T10" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U10" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V10" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1527,7 +1491,7 @@
         <v>27</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="F11" s="16">
         <v>48.429350999999997</v>
@@ -1548,10 +1512,10 @@
         <v>2611</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N11" s="17">
         <v>2605</v>
@@ -1560,7 +1524,7 @@
         <v>2408</v>
       </c>
       <c r="P11" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q11" s="17">
         <v>2305</v>
@@ -1569,16 +1533,16 @@
         <v>2408</v>
       </c>
       <c r="S11" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T11" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U11" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V11" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1586,7 +1550,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>64</v>
@@ -1595,7 +1559,7 @@
         <v>27</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="F12" s="16">
         <v>48.428482000000002</v>
@@ -1616,13 +1580,13 @@
         <v>2509</v>
       </c>
       <c r="L12" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N12" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O12" s="17">
         <v>2206</v>
@@ -1637,16 +1601,16 @@
         <v>2206</v>
       </c>
       <c r="S12" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T12" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U12" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V12" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1663,7 +1627,7 @@
         <v>27</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="F13" s="16">
         <v>48.427894000000002</v>
@@ -1684,13 +1648,13 @@
         <v>2302</v>
       </c>
       <c r="L13" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N13" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O13" s="17">
         <v>2001</v>
@@ -1705,16 +1669,16 @@
         <v>2001</v>
       </c>
       <c r="S13" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T13" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U13" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V13" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1722,7 +1686,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>64</v>
@@ -1731,7 +1695,7 @@
         <v>27</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="F14" s="16">
         <v>48.427315999999998</v>
@@ -1752,13 +1716,13 @@
         <v>2511</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M14" s="17">
         <v>2600</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O14" s="17">
         <v>2106</v>
@@ -1773,16 +1737,16 @@
         <v>2106</v>
       </c>
       <c r="S14" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T14" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U14" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V14" s="22" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1799,7 +1763,7 @@
         <v>27</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="F15" s="16">
         <v>48.426462999999998</v>
@@ -1820,13 +1784,13 @@
         <v>2808</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M15" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N15" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O15" s="17">
         <v>2509</v>
@@ -1837,20 +1801,20 @@
       <c r="Q15" s="17">
         <v>2606</v>
       </c>
-      <c r="R15" s="17" t="s">
-        <v>77</v>
+      <c r="R15" s="17">
+        <v>2506</v>
       </c>
       <c r="S15" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T15" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U15" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V15" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1858,7 +1822,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>64</v>
@@ -1867,7 +1831,7 @@
         <v>27</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F16" s="16">
         <v>48.425887000000003</v>
@@ -1888,13 +1852,13 @@
         <v>2904</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M16" s="17">
         <v>3000</v>
       </c>
       <c r="N16" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O16" s="17">
         <v>2304</v>
@@ -1909,16 +1873,16 @@
         <v>2304</v>
       </c>
       <c r="S16" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T16" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U16" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V16" s="22" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1935,7 +1899,7 @@
         <v>27</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F17" s="16">
         <v>48.425317</v>
@@ -1956,13 +1920,13 @@
         <v>2902</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M17" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N17" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O17" s="17">
         <v>2505</v>
@@ -1973,20 +1937,20 @@
       <c r="Q17" s="17">
         <v>2511</v>
       </c>
-      <c r="R17" s="17" t="s">
-        <v>81</v>
+      <c r="R17" s="17">
+        <v>2411</v>
       </c>
       <c r="S17" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="T17" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U17" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V17" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2003,7 +1967,7 @@
         <v>27</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F18" s="16">
         <v>48.424899000000003</v>
@@ -2015,7 +1979,7 @@
         <v>66</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J18" s="17">
         <v>2508</v>
@@ -2024,13 +1988,13 @@
         <v>2500</v>
       </c>
       <c r="L18" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M18" s="17">
         <v>2510</v>
       </c>
       <c r="N18" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O18" s="17">
         <v>2304</v>
@@ -2039,22 +2003,22 @@
         <v>2209</v>
       </c>
       <c r="Q18" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="R18" s="17" t="s">
-        <v>80</v>
+        <v>73</v>
+      </c>
+      <c r="R18" s="17">
+        <v>2108</v>
       </c>
       <c r="S18" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T18" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U18" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V18" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2071,7 +2035,7 @@
         <v>27</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F19" s="16">
         <v>48.424912999999997</v>
@@ -2083,7 +2047,7 @@
         <v>66</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J19" s="17">
         <v>2200</v>
@@ -2092,13 +2056,13 @@
         <v>2105</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M19" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N19" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O19" s="17">
         <v>1806</v>
@@ -2113,16 +2077,16 @@
         <v>1806</v>
       </c>
       <c r="S19" s="22" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="T19" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U19" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V19" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2130,7 +2094,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>64</v>
@@ -2139,7 +2103,7 @@
         <v>27</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F20" s="16">
         <v>48.424964000000003</v>
@@ -2151,22 +2115,22 @@
         <v>66</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K20" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L20" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M20" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N20" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O20" s="17">
         <v>2400</v>
@@ -2177,20 +2141,20 @@
       <c r="Q20" s="17">
         <v>2404</v>
       </c>
-      <c r="R20" s="17" t="s">
-        <v>84</v>
+      <c r="R20" s="17">
+        <v>2304</v>
       </c>
       <c r="S20" s="22" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="T20" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U20" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V20" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2207,7 +2171,7 @@
         <v>27</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F21" s="16">
         <v>48.424649000000002</v>
@@ -2219,22 +2183,22 @@
         <v>66</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K21" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L21" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M21" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N21" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O21" s="17">
         <v>1910</v>
@@ -2249,16 +2213,16 @@
         <v>1910</v>
       </c>
       <c r="S21" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T21" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U21" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V21" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2266,7 +2230,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>64</v>
@@ -2275,7 +2239,7 @@
         <v>27</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F22" s="16">
         <v>48.424443684700002</v>
@@ -2287,7 +2251,7 @@
         <v>66</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J22" s="17">
         <v>2505</v>
@@ -2296,13 +2260,13 @@
         <v>2500</v>
       </c>
       <c r="L22" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M22" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N22" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O22" s="17">
         <v>2210</v>
@@ -2313,20 +2277,20 @@
       <c r="Q22" s="17">
         <v>2303</v>
       </c>
-      <c r="R22" s="17" t="s">
-        <v>86</v>
+      <c r="R22" s="17">
+        <v>2101</v>
       </c>
       <c r="S22" s="22" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="T22" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U22" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V22" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2334,7 +2298,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>64</v>
@@ -2343,7 +2307,7 @@
         <v>27</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F23" s="16">
         <v>48.424171000000001</v>
@@ -2355,22 +2319,22 @@
         <v>66</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K23" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L23" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M23" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N23" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O23" s="17">
         <v>2409</v>
@@ -2385,16 +2349,16 @@
         <v>2409</v>
       </c>
       <c r="S23" s="22" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="T23" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U23" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V23" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2411,7 +2375,7 @@
         <v>27</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F24" s="16">
         <v>48.423363000000002</v>
@@ -2426,19 +2390,19 @@
         <v>2700</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K24" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L24" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M24" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N24" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O24" s="17">
         <v>2107</v>
@@ -2453,16 +2417,16 @@
         <v>2107</v>
       </c>
       <c r="S24" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T24" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U24" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V24" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2470,7 +2434,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>64</v>
@@ -2479,7 +2443,7 @@
         <v>27</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F25" s="16">
         <v>48.422941999999999</v>
@@ -2491,22 +2455,22 @@
         <v>66</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K25" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L25" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M25" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N25" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O25" s="17">
         <v>1910</v>
@@ -2521,16 +2485,16 @@
         <v>1910</v>
       </c>
       <c r="S25" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T25" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U25" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V25" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2547,7 +2511,7 @@
         <v>27</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F26" s="16">
         <v>48.422603000000002</v>
@@ -2562,19 +2526,19 @@
         <v>2508</v>
       </c>
       <c r="J26" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L26" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M26" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N26" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O26" s="17">
         <v>2305</v>
@@ -2585,20 +2549,20 @@
       <c r="Q26" s="17">
         <v>2400</v>
       </c>
-      <c r="R26" s="17" t="s">
-        <v>89</v>
+      <c r="R26" s="17">
+        <v>2104</v>
       </c>
       <c r="S26" s="22" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="T26" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U26" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V26" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2615,7 +2579,7 @@
         <v>27</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F27" s="16">
         <v>48.422683745500002</v>
@@ -2636,13 +2600,13 @@
         <v>2404</v>
       </c>
       <c r="L27" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M27" s="17">
         <v>2502</v>
       </c>
       <c r="N27" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O27" s="17">
         <v>2001</v>
@@ -2657,16 +2621,16 @@
         <v>2001</v>
       </c>
       <c r="S27" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T27" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U27" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V27" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2683,7 +2647,7 @@
         <v>27</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F28" s="16">
         <v>48.422690865500002</v>
@@ -2704,13 +2668,13 @@
         <v>2700</v>
       </c>
       <c r="L28" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M28" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N28" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O28" s="17">
         <v>2300</v>
@@ -2721,20 +2685,20 @@
       <c r="Q28" s="17">
         <v>2304</v>
       </c>
-      <c r="R28" s="17" t="s">
-        <v>91</v>
+      <c r="R28" s="17">
+        <v>2204</v>
       </c>
       <c r="S28" s="22" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="T28" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U28" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V28" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2751,7 +2715,7 @@
         <v>27</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F29" s="16">
         <v>48.422675290500003</v>
@@ -2772,13 +2736,13 @@
         <v>2800</v>
       </c>
       <c r="L29" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M29" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N29" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O29" s="17">
         <v>2503</v>
@@ -2787,22 +2751,22 @@
         <v>2405</v>
       </c>
       <c r="Q29" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R29" s="17" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="S29" s="22" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="T29" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U29" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V29" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2810,7 +2774,7 @@
         <v>21</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>64</v>
@@ -2819,7 +2783,7 @@
         <v>27</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F30" s="16">
         <v>48.422679518000002</v>
@@ -2840,13 +2804,13 @@
         <v>2800</v>
       </c>
       <c r="L30" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M30" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N30" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O30" s="17">
         <v>2405</v>
@@ -2855,22 +2819,22 @@
         <v>2400</v>
       </c>
       <c r="Q30" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R30" s="17">
         <v>2405</v>
       </c>
       <c r="S30" s="22" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="T30" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U30" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V30" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2878,7 +2842,7 @@
         <v>22</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>64</v>
@@ -2887,7 +2851,7 @@
         <v>27</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F31" s="16">
         <v>48.422663999999997</v>
@@ -2908,13 +2872,13 @@
         <v>2405</v>
       </c>
       <c r="L31" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M31" s="17">
         <v>2408</v>
       </c>
       <c r="N31" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O31" s="17">
         <v>2202</v>
@@ -2923,22 +2887,22 @@
         <v>2106</v>
       </c>
       <c r="Q31" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R31" s="17">
         <v>2202</v>
       </c>
       <c r="S31" s="22" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="T31" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U31" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V31" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2955,7 +2919,7 @@
         <v>27</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F32" s="16">
         <v>48.422173999999998</v>
@@ -2976,19 +2940,19 @@
         <v>2200</v>
       </c>
       <c r="L32" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M32" s="17">
         <v>2300</v>
       </c>
       <c r="N32" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O32" s="17">
         <v>1803</v>
       </c>
       <c r="P32" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q32" s="17">
         <v>1903</v>
@@ -2997,16 +2961,16 @@
         <v>1803</v>
       </c>
       <c r="S32" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T32" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U32" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V32" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3023,7 +2987,7 @@
         <v>27</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F33" s="16">
         <v>48.421857000000003</v>
@@ -3044,19 +3008,19 @@
         <v>2201</v>
       </c>
       <c r="L33" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M33" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N33" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O33" s="17">
         <v>1801</v>
       </c>
       <c r="P33" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q33" s="17">
         <v>1904</v>
@@ -3065,16 +3029,16 @@
         <v>1801</v>
       </c>
       <c r="S33" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T33" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U33" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V33" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3091,7 +3055,7 @@
         <v>27</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F34" s="16">
         <v>48.421419999999998</v>
@@ -3112,19 +3076,19 @@
         <v>2400</v>
       </c>
       <c r="L34" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M34" s="17">
         <v>2503</v>
       </c>
       <c r="N34" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O34" s="17">
         <v>1800</v>
       </c>
       <c r="P34" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q34" s="17">
         <v>1808</v>
@@ -3133,16 +3097,16 @@
         <v>1800</v>
       </c>
       <c r="S34" s="22" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="T34" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U34" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V34" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3159,7 +3123,7 @@
         <v>27</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F35" s="16">
         <v>48.421004000000003</v>
@@ -3180,10 +3144,10 @@
         <v>2105</v>
       </c>
       <c r="L35" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M35" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N35" s="17">
         <v>2100</v>
@@ -3192,7 +3156,7 @@
         <v>1700</v>
       </c>
       <c r="P35" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q35" s="17">
         <v>1802</v>
@@ -3201,16 +3165,16 @@
         <v>1700</v>
       </c>
       <c r="S35" s="22" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="T35" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U35" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V35" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3227,7 +3191,7 @@
         <v>27</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F36" s="16">
         <v>48.420662</v>
@@ -3248,19 +3212,19 @@
         <v>2007</v>
       </c>
       <c r="L36" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M36" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N36" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O36" s="17">
         <v>1608</v>
       </c>
       <c r="P36" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q36" s="17">
         <v>1708</v>
@@ -3269,16 +3233,16 @@
         <v>1608</v>
       </c>
       <c r="S36" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T36" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U36" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V36" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3286,7 +3250,7 @@
         <v>28</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>63</v>
@@ -3295,7 +3259,7 @@
         <v>27</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F37" s="16">
         <v>48.420259999999999</v>
@@ -3316,10 +3280,10 @@
         <v>2102</v>
       </c>
       <c r="L37" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M37" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N37" s="17">
         <v>2011</v>
@@ -3328,25 +3292,25 @@
         <v>1706</v>
       </c>
       <c r="P37" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q37" s="17">
         <v>1809</v>
       </c>
-      <c r="R37" s="17" t="s">
-        <v>99</v>
+      <c r="R37" s="17">
+        <v>1608</v>
       </c>
       <c r="S37" s="22" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="T37" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U37" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V37" s="22" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3363,7 +3327,7 @@
         <v>27</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F38" s="16">
         <v>48.419958999999999</v>
@@ -3384,19 +3348,19 @@
         <v>2402</v>
       </c>
       <c r="L38" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M38" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N38" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O38" s="17">
         <v>1910</v>
       </c>
       <c r="P38" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q38" s="17">
         <v>2010</v>
@@ -3405,16 +3369,16 @@
         <v>1910</v>
       </c>
       <c r="S38" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T38" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U38" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V38" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3431,7 +3395,7 @@
         <v>27</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F39" s="16">
         <v>48.419598000000001</v>
@@ -3452,7 +3416,7 @@
         <v>2210</v>
       </c>
       <c r="L39" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M39" s="17">
         <v>2208</v>
@@ -3464,30 +3428,30 @@
         <v>2000</v>
       </c>
       <c r="P39" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q39" s="17">
         <v>2004</v>
       </c>
-      <c r="R39" s="17" t="s">
-        <v>101</v>
+      <c r="R39" s="17">
+        <v>1804</v>
       </c>
       <c r="S39" s="22" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="T39" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U39" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V39" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B40" s="21" t="s">
         <v>59</v>
@@ -3499,7 +3463,7 @@
         <v>27</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F40" s="16">
         <v>48.419241</v>
@@ -3520,13 +3484,13 @@
         <v>2503</v>
       </c>
       <c r="L40" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M40" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N40" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O40" s="17">
         <v>2105</v>
@@ -3541,16 +3505,16 @@
         <v>2105</v>
       </c>
       <c r="S40" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T40" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U40" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V40" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3558,7 +3522,7 @@
         <v>31</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>64</v>
@@ -3567,7 +3531,7 @@
         <v>27</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F41" s="16">
         <v>48.422677999999998</v>
@@ -3582,19 +3546,19 @@
         <v>2902</v>
       </c>
       <c r="J41" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K41" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L41" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M41" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N41" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O41" s="17">
         <v>2004</v>
@@ -3603,22 +3567,22 @@
         <v>1709</v>
       </c>
       <c r="Q41" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R41" s="17">
         <v>2004</v>
       </c>
       <c r="S41" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T41" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U41" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V41" s="22" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3626,7 +3590,7 @@
         <v>32</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>64</v>
@@ -3635,7 +3599,7 @@
         <v>27</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F42" s="16">
         <v>48.422384999999998</v>
@@ -3656,13 +3620,13 @@
         <v>2700</v>
       </c>
       <c r="L42" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M42" s="17">
         <v>2801</v>
       </c>
       <c r="N42" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O42" s="17">
         <v>2204</v>
@@ -3671,22 +3635,22 @@
         <v>2104</v>
       </c>
       <c r="Q42" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R42" s="17">
         <v>2204</v>
       </c>
       <c r="S42" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T42" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U42" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V42" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3703,7 +3667,7 @@
         <v>27</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F43" s="16">
         <v>48.421937</v>
@@ -3724,13 +3688,13 @@
         <v>2401</v>
       </c>
       <c r="L43" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M43" s="17">
         <v>2500</v>
       </c>
       <c r="N43" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O43" s="17">
         <v>2110</v>
@@ -3739,22 +3703,22 @@
         <v>2009</v>
       </c>
       <c r="Q43" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R43" s="17">
         <v>2110</v>
       </c>
       <c r="S43" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T43" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U43" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V43" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3771,7 +3735,7 @@
         <v>27</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F44" s="16">
         <v>48.421419999999998</v>
@@ -3792,13 +3756,13 @@
         <v>2304</v>
       </c>
       <c r="L44" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M44" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N44" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O44" s="17">
         <v>2004</v>
@@ -3807,22 +3771,22 @@
         <v>2006</v>
       </c>
       <c r="Q44" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="R44" s="17" t="s">
-        <v>103</v>
+        <v>73</v>
+      </c>
+      <c r="R44" s="17">
+        <v>2000</v>
       </c>
       <c r="S44" s="22" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="T44" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U44" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V44" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3830,7 +3794,7 @@
         <v>35</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>64</v>
@@ -3839,7 +3803,7 @@
         <v>27</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F45" s="16">
         <v>48.421143000000001</v>
@@ -3860,13 +3824,13 @@
         <v>2510</v>
       </c>
       <c r="L45" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M45" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N45" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O45" s="17">
         <v>2208</v>
@@ -3875,22 +3839,22 @@
         <v>2101</v>
       </c>
       <c r="Q45" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R45" s="17">
         <v>2208</v>
       </c>
       <c r="S45" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T45" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U45" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V45" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3898,7 +3862,7 @@
         <v>36</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>64</v>
@@ -3907,7 +3871,7 @@
         <v>27</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F46" s="16">
         <v>48.420833999999999</v>
@@ -3928,13 +3892,13 @@
         <v>2504</v>
       </c>
       <c r="L46" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M46" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N46" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O46" s="17">
         <v>2211</v>
@@ -3943,22 +3907,22 @@
         <v>2201</v>
       </c>
       <c r="Q46" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R46" s="17">
         <v>2211</v>
       </c>
       <c r="S46" s="22" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="T46" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U46" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V46" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3975,7 +3939,7 @@
         <v>27</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F47" s="16">
         <v>48.420555999999998</v>
@@ -3996,13 +3960,13 @@
         <v>2509</v>
       </c>
       <c r="L47" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M47" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N47" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O47" s="17">
         <v>2008</v>
@@ -4011,22 +3975,22 @@
         <v>2000</v>
       </c>
       <c r="Q47" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R47" s="17">
         <v>2008</v>
       </c>
       <c r="S47" s="22" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="T47" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U47" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V47" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4034,7 +3998,7 @@
         <v>38</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>64</v>
@@ -4043,19 +4007,19 @@
         <v>27</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="H48" s="15" t="s">
         <v>66</v>
       </c>
       <c r="I48" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J48" s="17">
         <v>2505</v>
@@ -4064,13 +4028,13 @@
         <v>2409</v>
       </c>
       <c r="L48" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M48" s="17">
         <v>2406</v>
       </c>
       <c r="N48" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O48" s="17">
         <v>2209</v>
@@ -4079,22 +4043,22 @@
         <v>2200</v>
       </c>
       <c r="Q48" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="R48" s="17" t="s">
-        <v>129</v>
+        <v>73</v>
+      </c>
+      <c r="R48" s="17">
+        <v>2100</v>
       </c>
       <c r="S48" s="22" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="T48" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U48" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V48" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="6:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>